<commit_message>
fix a few links
fix a few links
</commit_message>
<xml_diff>
--- a/.files/bookmarks_new_2024-04-04.xlsx
+++ b/.files/bookmarks_new_2024-04-04.xlsx
@@ -8,18 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cassi\Documents\GitHub\AB-RCSC\RCSC-WildCAM_Remote-Camera-Survey-Guidelines-and-Metadata-Standards\.files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56CD7F1D-F168-4892-AF04-2E601DF6C2B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E432A35-7871-4A94-980B-2A5F568A6AFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{FA56EECE-27D8-44D9-BFF7-2AE0F7DB9A15}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{FA56EECE-27D8-44D9-BFF7-2AE0F7DB9A15}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{92210062-A3D4-41AC-AED9-23F967524134}"/>
   </bookViews>
   <sheets>
     <sheet name="keys" sheetId="4" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="13" r:id="rId2"/>
-    <sheet name="errors" sheetId="12" r:id="rId3"/>
-    <sheet name="Sheet5" sheetId="5" r:id="rId4"/>
+    <sheet name="wildtrax" sheetId="14" r:id="rId3"/>
+    <sheet name="errors" sheetId="12" r:id="rId4"/>
+    <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">keys!$A$1:$I$388</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet1!$A$1:$G$86</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3009" uniqueCount="1353">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3236" uniqueCount="1432">
   <si>
     <t>trigger_event</t>
   </si>
@@ -4089,21 +4092,6 @@
     <t>battery_percent</t>
   </si>
   <si>
-    <t>new_cam_id</t>
-  </si>
-  <si>
-    <t>new_cam_make</t>
-  </si>
-  <si>
-    <t>new_cam_model</t>
-  </si>
-  <si>
-    <t>new_cam_serial</t>
-  </si>
-  <si>
-    <t>new_sd_card_id</t>
-  </si>
-  <si>
     <t>set_trig_modes</t>
   </si>
   <si>
@@ -4197,32 +4185,284 @@
     <t>Tag</t>
   </si>
   <si>
-    <t>Adult</t>
-  </si>
-  <si>
-    <t>Juvenile</t>
-  </si>
-  <si>
-    <t>Subadult</t>
-  </si>
-  <si>
-    <t>Subadult - Yearling</t>
-  </si>
-  <si>
-    <t>Subadult - Young of Year</t>
-  </si>
-  <si>
     <t>location</t>
   </si>
   <si>
-    <t>visit_start_date_time</t>
+    <t>project_id</t>
+  </si>
+  <si>
+    <t>location_id</t>
+  </si>
+  <si>
+    <t>equipment_make</t>
+  </si>
+  <si>
+    <t>equipment_model</t>
+  </si>
+  <si>
+    <t>equipment_serial</t>
+  </si>
+  <si>
+    <t>image_set_status</t>
+  </si>
+  <si>
+    <t>image_set_count_motion</t>
+  </si>
+  <si>
+    <t>image_set_count_total</t>
+  </si>
+  <si>
+    <t>image_set_count_timelapse</t>
+  </si>
+  <si>
+    <t>image_set_id</t>
+  </si>
+  <si>
+    <t>image_set_url</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>organization</t>
+  </si>
+  <si>
+    <t>location_buffer_m</t>
+  </si>
+  <si>
+    <t>latitude</t>
+  </si>
+  <si>
+    <t>longitude</t>
+  </si>
+  <si>
+    <t>location_visibility</t>
+  </si>
+  <si>
+    <t>elevation</t>
+  </si>
+  <si>
+    <t>location_comments</t>
+  </si>
+  <si>
+    <t>image_id</t>
+  </si>
+  <si>
+    <t>image_date_time</t>
+  </si>
+  <si>
+    <t>source_file_name</t>
+  </si>
+  <si>
+    <t>image_fire</t>
+  </si>
+  <si>
+    <t>image_nice</t>
+  </si>
+  <si>
+    <t>image_malfunction</t>
+  </si>
+  <si>
+    <t>image_fov</t>
+  </si>
+  <si>
+    <t>image_snow</t>
+  </si>
+  <si>
+    <t>image_snow_depth_m</t>
+  </si>
+  <si>
+    <t>image_water_depth_m</t>
+  </si>
+  <si>
+    <t>image_exif_temperature</t>
+  </si>
+  <si>
+    <t>image_exif_sequence</t>
+  </si>
+  <si>
+    <t>image_is_blurred</t>
+  </si>
+  <si>
+    <t>media_url</t>
+  </si>
+  <si>
+    <t>image_in_wildtrax</t>
+  </si>
+  <si>
+    <t>image_comments</t>
+  </si>
+  <si>
+    <t>species_scientific_name</t>
+  </si>
+  <si>
+    <t>species_common_name</t>
+  </si>
+  <si>
+    <t>behaviours</t>
+  </si>
+  <si>
+    <t>health_diseases</t>
+  </si>
+  <si>
+    <t>coat_colours</t>
+  </si>
+  <si>
+    <t>coat_attributes</t>
+  </si>
+  <si>
+    <t>tine_attributes</t>
+  </si>
+  <si>
+    <t>direction_travel</t>
+  </si>
+  <si>
+    <t>has_collar</t>
+  </si>
+  <si>
+    <t>has_eartag</t>
+  </si>
+  <si>
+    <t>ihf</t>
+  </si>
+  <si>
+    <t>observer</t>
+  </si>
+  <si>
+    <t>observer_id</t>
+  </si>
+  <si>
+    <t>tag_comments</t>
+  </si>
+  <si>
+    <t>tag_needs_review</t>
+  </si>
+  <si>
+    <t>tag_is_verified</t>
+  </si>
+  <si>
+    <t>tag_id</t>
+  </si>
+  <si>
+    <t>project_status</t>
+  </si>
+  <si>
+    <t>project_results</t>
+  </si>
+  <si>
+    <t>report</t>
+  </si>
+  <si>
+    <t>note</t>
+  </si>
+  <si>
+    <t>pi???</t>
+  </si>
+  <si>
+    <t>field</t>
+  </si>
+  <si>
+    <t>image_report</t>
+  </si>
+  <si>
+    <t>main_report</t>
+  </si>
+  <si>
+    <t>image_set_report</t>
+  </si>
+  <si>
+    <t>location_report</t>
+  </si>
+  <si>
+    <t>project_report</t>
+  </si>
+  <si>
+    <t>accessMethod</t>
+  </si>
+  <si>
+    <t>visits</t>
+  </si>
+  <si>
+    <t>comments</t>
+  </si>
+  <si>
+    <t>ifelse(equipment$serialNumber == , equipment$code, NA(</t>
+  </si>
+  <si>
+    <t>pgadmin</t>
+  </si>
+  <si>
+    <t>camera.image_meta</t>
+  </si>
+  <si>
+    <t>im_flash</t>
+  </si>
+  <si>
+    <t>where</t>
+  </si>
+  <si>
+    <t>common.lu_location_visit_access_method</t>
+  </si>
+  <si>
+    <t>lvam_type</t>
+  </si>
+  <si>
+    <t>common.lu_location_equipment_mount</t>
+  </si>
+  <si>
+    <t>lem_type</t>
+  </si>
+  <si>
+    <t>ignore</t>
+  </si>
+  <si>
+    <t>common.lu_land_feature</t>
+  </si>
+  <si>
+    <t>land_feature_type</t>
+  </si>
+  <si>
+    <t>common.lu_location_equipment_target</t>
+  </si>
+  <si>
+    <t>le_tar_type</t>
+  </si>
+  <si>
+    <t>le_trigger_seconds_between_pictures</t>
+  </si>
+  <si>
+    <t>location_equipment</t>
+  </si>
+  <si>
+    <t>le_direction_degrees</t>
+  </si>
+  <si>
+    <t>le_quiet_period_seconds</t>
+  </si>
+  <si>
+    <t>le_walk_test_distance_m</t>
+  </si>
+  <si>
+    <t>le_walk_test_height_m</t>
+  </si>
+  <si>
+    <t>le_working_test_done</t>
+  </si>
+  <si>
+    <t>le_height_meters</t>
+  </si>
+  <si>
+    <t>sort</t>
+  </si>
+  <si>
+    <t>[]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12">
+  <fonts count="28">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4295,8 +4535,128 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Aptos Display"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="19">
+  <fills count="49">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4401,12 +4761,179 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFF3FF"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -4430,25 +4957,160 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
-        <color rgb="FFBFBFBF"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FFBFBFBF"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FFBFBFBF"/>
+        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="44" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="45" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="46" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="47" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="48" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -4508,20 +5170,176 @@
     <xf numFmtId="0" fontId="10" fillId="17" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="44">
+    <cellStyle name="20% - Accent1" xfId="21" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="25" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="29" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="33" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="37" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="41" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="22" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="26" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="30" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="34" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="38" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="42" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="23" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="27" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="31" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="35" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="39" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="43" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="20" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="24" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="28" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="32" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="36" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="40" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="9" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="13" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="15" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="18" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="8" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="4" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="5" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="6" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="7" builtinId="19" customBuiltin="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Input" xfId="11" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="14" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="10" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{E7A5A5F8-22F3-44E9-B3C0-2A8A36208EEB}"/>
+    <cellStyle name="Note" xfId="17" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="12" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="3" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="19" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="16" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="23">
+  <dxfs count="113">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF3F3F3"/>
+          <bgColor rgb="FFF3F3F3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF3F3F3"/>
+          <bgColor rgb="FFF3F3F3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF3F3F3"/>
+          <bgColor rgb="FFF3F3F3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -4571,9 +5389,6 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FFECECEC"/>
@@ -4608,8 +5423,656 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF9999"/>
+          <bgColor rgb="FFFF9999"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
           <fgColor rgb="FFECECEC"/>
           <bgColor rgb="FFECECEC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF3F3F3"/>
+          <bgColor rgb="FFF3F3F3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF3F3F3"/>
+          <bgColor rgb="FFF3F3F3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF3F3F3"/>
+          <bgColor rgb="FFF3F3F3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF3F3F3"/>
+          <bgColor rgb="FFF3F3F3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF3F3F3"/>
+          <bgColor rgb="FFF3F3F3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF3F3F3"/>
+          <bgColor rgb="FFF3F3F3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF3F3F3"/>
+          <bgColor rgb="FFF3F3F3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF3F3F3"/>
+          <bgColor rgb="FFF3F3F3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF3F3F3"/>
+          <bgColor rgb="FFF3F3F3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF3F3F3"/>
+          <bgColor rgb="FFF3F3F3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF3F3F3"/>
+          <bgColor rgb="FFF3F3F3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF3F3F3"/>
+          <bgColor rgb="FFF3F3F3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF3F3F3"/>
+          <bgColor rgb="FFF3F3F3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF3F3F3"/>
+          <bgColor rgb="FFF3F3F3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF3F3F3"/>
+          <bgColor rgb="FFF3F3F3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF3F3F3"/>
+          <bgColor rgb="FFF3F3F3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF3F3F3"/>
+          <bgColor rgb="FFF3F3F3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF3F3F3"/>
+          <bgColor rgb="FFF3F3F3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF3F3F3"/>
+          <bgColor rgb="FFF3F3F3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF3F3F3"/>
+          <bgColor rgb="FFF3F3F3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF3F3F3"/>
+          <bgColor rgb="FFF3F3F3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF3F3F3"/>
+          <bgColor rgb="FFF3F3F3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF3F3F3"/>
+          <bgColor rgb="FFF3F3F3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF3F3F3"/>
+          <bgColor rgb="FFF3F3F3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF3F3F3"/>
+          <bgColor rgb="FFF3F3F3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF3F3F3"/>
+          <bgColor rgb="FFF3F3F3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
         </patternFill>
       </fill>
     </dxf>
@@ -5056,6 +6519,7 @@
       <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -14821,7 +16285,7 @@
   </autoFilter>
   <phoneticPr fontId="4" type="noConversion"/>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="containsText" dxfId="22" priority="1" operator="containsText" text="_id">
+    <cfRule type="containsText" dxfId="112" priority="1" operator="containsText" text="_id">
       <formula>NOT(ISERROR(SEARCH("_id",E1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14888,551 +16352,1786 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E5F9EF8-3CBA-4CCB-8F7D-668C099D13C0}">
-  <dimension ref="A1:B97"/>
+  <dimension ref="A1:P86"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="F41" sqref="F41"/>
+    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="1">
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F70" sqref="F70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="30.85546875" style="25" customWidth="1"/>
-    <col min="2" max="2" width="46" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="44"/>
+    <col min="2" max="2" width="41.140625" style="23" customWidth="1"/>
+    <col min="3" max="3" width="9" style="23" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" style="41" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="32.85546875" customWidth="1"/>
+    <col min="7" max="7" width="21.5703125" customWidth="1"/>
+    <col min="8" max="8" width="10.5703125" customWidth="1"/>
+    <col min="19" max="19" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:8">
+      <c r="A1" s="44" t="s">
+        <v>1430</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>1276</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="8" t="s">
+      <c r="C1" s="33" t="s">
+        <v>1417</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>1396</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1399</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1409</v>
+      </c>
+      <c r="G1" t="s">
+        <v>1412</v>
+      </c>
+      <c r="H1" t="s">
+        <v>1397</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="44">
+        <v>21</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>710</v>
+      </c>
+      <c r="C2" s="30"/>
+      <c r="D2" s="38" t="s">
+        <v>1406</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1405</v>
+      </c>
+      <c r="F2" t="s">
+        <v>1414</v>
+      </c>
+      <c r="G2" s="30" t="s">
+        <v>1413</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="44">
+        <v>76</v>
+      </c>
+      <c r="B3" s="22" t="s">
+        <v>112</v>
+      </c>
+      <c r="C3" s="36"/>
+      <c r="D3" s="37" t="s">
+        <v>1401</v>
+      </c>
+      <c r="E3" s="36" t="s">
+        <v>112</v>
+      </c>
+      <c r="H3" s="44"/>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="44">
+        <v>78</v>
+      </c>
+      <c r="B4" s="22" t="s">
+        <v>113</v>
+      </c>
+      <c r="C4" s="36"/>
+      <c r="D4" s="37" t="s">
+        <v>1401</v>
+      </c>
+      <c r="E4" s="36" t="s">
+        <v>1379</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="44">
+        <v>29</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="C5" s="35"/>
+      <c r="D5" s="38" t="s">
+        <v>1406</v>
+      </c>
+      <c r="E5" s="44" t="s">
+        <v>1407</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="44">
+        <v>30</v>
+      </c>
+      <c r="B6" s="18" t="s">
+        <v>1300</v>
+      </c>
+      <c r="C6" s="35"/>
+      <c r="D6" s="38" t="s">
+        <v>1406</v>
+      </c>
+      <c r="E6" s="44" t="s">
+        <v>1407</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="44">
+        <v>31</v>
+      </c>
+      <c r="B7" s="18" t="s">
+        <v>139</v>
+      </c>
+      <c r="C7" s="35"/>
+      <c r="D7" s="38" t="s">
+        <v>1406</v>
+      </c>
+      <c r="E7" s="44" t="s">
+        <v>1407</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="44">
+        <v>26</v>
+      </c>
+      <c r="B8" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="C8" s="35"/>
+      <c r="D8" s="38" t="s">
+        <v>1406</v>
+      </c>
+      <c r="E8" s="44" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="44">
+        <v>33</v>
+      </c>
+      <c r="B9" s="20" t="s">
+        <v>1302</v>
+      </c>
+      <c r="C9" s="32"/>
+      <c r="D9" s="39" t="s">
+        <v>1402</v>
+      </c>
+      <c r="E9" s="44" t="s">
+        <v>1344</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="44">
+        <v>34</v>
+      </c>
+      <c r="B10" s="20" t="s">
+        <v>1303</v>
+      </c>
+      <c r="C10" s="32"/>
+      <c r="D10" s="39" t="s">
+        <v>1402</v>
+      </c>
+      <c r="E10" s="44" t="s">
+        <v>1345</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="44">
+        <v>35</v>
+      </c>
+      <c r="B11" s="20" t="s">
+        <v>1304</v>
+      </c>
+      <c r="C11" s="32"/>
+      <c r="D11" s="39" t="s">
+        <v>1402</v>
+      </c>
+      <c r="E11" s="44" t="s">
+        <v>1346</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="44">
+        <v>83</v>
+      </c>
+      <c r="B12" s="22" t="s">
+        <v>1337</v>
+      </c>
+      <c r="C12" s="36"/>
+      <c r="D12" s="37" t="s">
+        <v>1400</v>
+      </c>
+      <c r="E12" s="44" t="s">
+        <v>1372</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="44">
+        <v>69</v>
+      </c>
+      <c r="B13" s="18" t="s">
+        <v>1330</v>
+      </c>
+      <c r="C13" s="35"/>
+      <c r="D13" s="39" t="s">
+        <v>1402</v>
+      </c>
+      <c r="E13" s="44" t="s">
+        <v>1349</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="44">
+        <v>68</v>
+      </c>
+      <c r="B14" s="18" t="s">
+        <v>1329</v>
+      </c>
+      <c r="C14" s="35"/>
+      <c r="D14" s="39" t="s">
+        <v>1402</v>
+      </c>
+      <c r="E14" s="44" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="44">
+        <v>67</v>
+      </c>
+      <c r="B15" s="18" t="s">
+        <v>1328</v>
+      </c>
+      <c r="C15" s="35"/>
+      <c r="D15" s="39" t="s">
+        <v>1402</v>
+      </c>
+      <c r="E15" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="44">
+        <v>75</v>
+      </c>
+      <c r="B16" s="22" t="s">
+        <v>142</v>
+      </c>
+      <c r="C16" s="36"/>
+      <c r="D16" s="37" t="s">
+        <v>1401</v>
+      </c>
+      <c r="E16" s="36" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16">
+      <c r="A17" s="44">
+        <v>15</v>
+      </c>
+      <c r="B17" s="16" t="s">
+        <v>1288</v>
+      </c>
+      <c r="C17" s="30"/>
+      <c r="D17" s="39" t="s">
+        <v>1403</v>
+      </c>
+      <c r="E17" s="44" t="s">
+        <v>1356</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16">
+      <c r="A18" s="44">
+        <v>14</v>
+      </c>
+      <c r="B18" s="15" t="s">
+        <v>1287</v>
+      </c>
+      <c r="C18" s="27"/>
+      <c r="D18" s="39" t="s">
+        <v>1403</v>
+      </c>
+      <c r="E18" s="44" t="s">
+        <v>1341</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16">
+      <c r="A19" s="44">
+        <v>22</v>
+      </c>
+      <c r="B19" s="16" t="s">
+        <v>1294</v>
+      </c>
+      <c r="C19" s="30"/>
+      <c r="D19" s="39" t="s">
+        <v>1403</v>
+      </c>
+      <c r="E19" s="44" t="s">
+        <v>1360</v>
+      </c>
+      <c r="F19" t="s">
+        <v>1416</v>
+      </c>
+      <c r="G19" t="s">
+        <v>1415</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16">
+      <c r="A20" s="44">
+        <v>16</v>
+      </c>
+      <c r="B20" s="16" t="s">
+        <v>1289</v>
+      </c>
+      <c r="C20" s="30"/>
+      <c r="D20" s="39" t="s">
+        <v>1403</v>
+      </c>
+      <c r="E20" s="44" t="s">
+        <v>1357</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16">
+      <c r="A21" s="44">
+        <v>2</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>1278</v>
+      </c>
+      <c r="C21" s="25"/>
+      <c r="D21" s="38" t="s">
+        <v>1353</v>
+      </c>
+      <c r="E21" s="38" t="s">
+        <v>1353</v>
+      </c>
+      <c r="G21" s="43"/>
+      <c r="H21" t="s">
+        <v>1398</v>
+      </c>
+      <c r="I21" s="43"/>
+      <c r="J21" s="43"/>
+      <c r="K21" s="43"/>
+      <c r="L21" s="43"/>
+      <c r="M21" s="43"/>
+      <c r="N21" s="43"/>
+      <c r="O21" s="43"/>
+      <c r="P21" s="43"/>
+    </row>
+    <row r="22" spans="1:16">
+      <c r="A22" s="44">
+        <v>3</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>1279</v>
+      </c>
+      <c r="C22" s="25"/>
+      <c r="D22" s="38" t="s">
+        <v>1353</v>
+      </c>
+      <c r="E22" s="38" t="s">
+        <v>1353</v>
+      </c>
+      <c r="G22" s="40"/>
+      <c r="H22" t="s">
+        <v>1398</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16">
+      <c r="A23" s="44">
+        <v>5</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" s="38" t="b">
+        <v>1</v>
+      </c>
+      <c r="D23" s="38" t="s">
+        <v>1353</v>
+      </c>
+      <c r="E23" s="38" t="s">
+        <v>1353</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16">
+      <c r="A24" s="44">
+        <v>6</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>1281</v>
+      </c>
+      <c r="C24" s="38" t="b">
+        <v>1</v>
+      </c>
+      <c r="D24" s="38" t="s">
+        <v>1353</v>
+      </c>
+      <c r="E24" s="38" t="s">
+        <v>1353</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16">
+      <c r="A25" s="44">
+        <v>7</v>
+      </c>
+      <c r="B25" s="12" t="s">
+        <v>1282</v>
+      </c>
+      <c r="C25" s="38" t="b">
+        <v>1</v>
+      </c>
+      <c r="D25" s="38" t="s">
+        <v>1353</v>
+      </c>
+      <c r="E25" s="38" t="s">
+        <v>1353</v>
+      </c>
+      <c r="G25" s="43"/>
+      <c r="I25" s="34"/>
+    </row>
+    <row r="26" spans="1:16">
+      <c r="A26" s="44">
+        <v>8</v>
+      </c>
+      <c r="B26" s="13" t="s">
+        <v>1283</v>
+      </c>
+      <c r="C26" s="38" t="b">
+        <v>1</v>
+      </c>
+      <c r="D26" s="38" t="s">
+        <v>1353</v>
+      </c>
+      <c r="E26" s="38" t="s">
+        <v>1353</v>
+      </c>
+      <c r="G26" s="43"/>
+      <c r="I26" s="43"/>
+    </row>
+    <row r="27" spans="1:16">
+      <c r="A27" s="44">
+        <v>9</v>
+      </c>
+      <c r="B27" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C27" s="38" t="b">
+        <v>1</v>
+      </c>
+      <c r="D27" s="38" t="s">
+        <v>1353</v>
+      </c>
+      <c r="E27" s="38" t="s">
+        <v>1353</v>
+      </c>
+      <c r="G27" s="43"/>
+      <c r="I27" s="43"/>
+    </row>
+    <row r="28" spans="1:16">
+      <c r="A28" s="44">
+        <v>10</v>
+      </c>
+      <c r="B28" s="13" t="s">
+        <v>1284</v>
+      </c>
+      <c r="C28" s="38" t="b">
+        <v>1</v>
+      </c>
+      <c r="D28" s="38" t="s">
+        <v>1353</v>
+      </c>
+      <c r="E28" s="38" t="s">
+        <v>1353</v>
+      </c>
+      <c r="G28" s="43"/>
+      <c r="I28" s="43"/>
+    </row>
+    <row r="29" spans="1:16">
+      <c r="A29" s="44">
+        <v>11</v>
+      </c>
+      <c r="B29" s="13" t="s">
+        <v>1285</v>
+      </c>
+      <c r="C29" s="38" t="b">
+        <v>1</v>
+      </c>
+      <c r="D29" s="38" t="s">
+        <v>1353</v>
+      </c>
+      <c r="E29" s="38" t="s">
+        <v>1353</v>
+      </c>
+      <c r="G29" s="43"/>
+      <c r="I29" s="43"/>
+    </row>
+    <row r="30" spans="1:16">
+      <c r="A30" s="44">
+        <v>13</v>
+      </c>
+      <c r="B30" s="14" t="s">
+        <v>1286</v>
+      </c>
+      <c r="C30" s="38" t="b">
+        <v>1</v>
+      </c>
+      <c r="D30" s="38" t="s">
+        <v>1353</v>
+      </c>
+      <c r="E30" s="38" t="s">
+        <v>1353</v>
+      </c>
+      <c r="G30" s="43"/>
+      <c r="I30" s="43"/>
+    </row>
+    <row r="31" spans="1:16">
+      <c r="A31" s="44">
+        <v>17</v>
+      </c>
+      <c r="B31" s="16" t="s">
+        <v>1290</v>
+      </c>
+      <c r="C31" s="38" t="b">
+        <v>1</v>
+      </c>
+      <c r="D31" s="38" t="s">
+        <v>1353</v>
+      </c>
+      <c r="E31" s="38" t="s">
+        <v>1353</v>
+      </c>
+      <c r="G31" s="43"/>
+      <c r="I31" s="43"/>
+    </row>
+    <row r="32" spans="1:16">
+      <c r="A32" s="44">
+        <v>18</v>
+      </c>
+      <c r="B32" s="16" t="s">
+        <v>1291</v>
+      </c>
+      <c r="C32" s="38" t="b">
+        <v>1</v>
+      </c>
+      <c r="D32" s="38" t="s">
+        <v>1353</v>
+      </c>
+      <c r="E32" s="38" t="s">
+        <v>1353</v>
+      </c>
+      <c r="G32" s="43"/>
+      <c r="I32" s="43"/>
+    </row>
+    <row r="33" spans="1:9">
+      <c r="A33" s="44">
+        <v>19</v>
+      </c>
+      <c r="B33" s="16" t="s">
+        <v>1292</v>
+      </c>
+      <c r="C33" s="38" t="b">
+        <v>1</v>
+      </c>
+      <c r="D33" s="38" t="s">
+        <v>1353</v>
+      </c>
+      <c r="E33" s="38" t="s">
+        <v>1353</v>
+      </c>
+      <c r="G33" s="43"/>
+      <c r="I33" s="43"/>
+    </row>
+    <row r="34" spans="1:9">
+      <c r="A34" s="44">
+        <v>20</v>
+      </c>
+      <c r="B34" s="16" t="s">
+        <v>1293</v>
+      </c>
+      <c r="C34" s="38" t="b">
+        <v>1</v>
+      </c>
+      <c r="D34" s="38" t="s">
+        <v>1353</v>
+      </c>
+      <c r="E34" s="38" t="s">
+        <v>1353</v>
+      </c>
+      <c r="G34" s="43"/>
+      <c r="I34" s="43"/>
+    </row>
+    <row r="35" spans="1:9">
+      <c r="A35" s="44">
+        <v>47</v>
+      </c>
+      <c r="B35" s="18" t="s">
+        <v>1311</v>
+      </c>
+      <c r="C35" s="38" t="b">
+        <v>1</v>
+      </c>
+      <c r="D35" s="38" t="s">
+        <v>1353</v>
+      </c>
+      <c r="E35" s="38" t="s">
+        <v>1353</v>
+      </c>
+      <c r="I35" s="43"/>
+    </row>
+    <row r="36" spans="1:9">
+      <c r="A36" s="44">
+        <v>66</v>
+      </c>
+      <c r="B36" s="20" t="s">
+        <v>1327</v>
+      </c>
+      <c r="C36" s="38" t="b">
+        <v>1</v>
+      </c>
+      <c r="D36" s="44" t="s">
+        <v>1353</v>
+      </c>
+      <c r="E36" s="44" t="s">
+        <v>1353</v>
+      </c>
+      <c r="I36" s="43"/>
+    </row>
+    <row r="37" spans="1:9">
+      <c r="A37" s="44">
+        <v>71</v>
+      </c>
+      <c r="B37" s="21" t="s">
+        <v>1332</v>
+      </c>
+      <c r="C37" s="29"/>
+      <c r="D37" s="44" t="s">
+        <v>1353</v>
+      </c>
+      <c r="E37" t="s">
+        <v>1353</v>
+      </c>
+      <c r="I37" s="43"/>
+    </row>
+    <row r="38" spans="1:9">
+      <c r="A38" s="44">
+        <v>79</v>
+      </c>
+      <c r="B38" s="22" t="s">
+        <v>144</v>
+      </c>
+      <c r="C38" s="36"/>
+      <c r="D38" s="44" t="s">
+        <v>1353</v>
+      </c>
+      <c r="E38" t="s">
+        <v>1353</v>
+      </c>
+      <c r="I38" s="43"/>
+    </row>
+    <row r="39" spans="1:9">
+      <c r="A39" s="44">
+        <v>82</v>
+      </c>
+      <c r="B39" s="22" t="s">
+        <v>1336</v>
+      </c>
+      <c r="C39" s="36"/>
+      <c r="D39" s="44" t="s">
+        <v>1353</v>
+      </c>
+      <c r="E39" t="s">
+        <v>1353</v>
+      </c>
+      <c r="I39" s="43"/>
+    </row>
+    <row r="40" spans="1:9">
+      <c r="A40" s="44">
+        <v>84</v>
+      </c>
+      <c r="B40" s="22" t="s">
+        <v>1338</v>
+      </c>
+      <c r="C40" s="36"/>
+      <c r="D40" s="44" t="s">
+        <v>1353</v>
+      </c>
+      <c r="E40" t="s">
+        <v>1353</v>
+      </c>
+      <c r="I40" s="43"/>
+    </row>
+    <row r="41" spans="1:9">
+      <c r="A41" s="44">
+        <v>73</v>
+      </c>
+      <c r="B41" s="22" t="s">
+        <v>114</v>
+      </c>
+      <c r="C41" s="36"/>
+      <c r="D41" s="37" t="s">
+        <v>1401</v>
+      </c>
+      <c r="E41" t="s">
+        <v>1388</v>
+      </c>
+      <c r="I41" s="43"/>
+    </row>
+    <row r="42" spans="1:9">
+      <c r="A42" s="44">
+        <v>1</v>
+      </c>
+      <c r="B42" s="8" t="s">
         <v>1277</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C42" s="42"/>
+      <c r="D42" s="39" t="s">
+        <v>1404</v>
+      </c>
+      <c r="E42" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="9" t="s">
-        <v>1278</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="9" t="s">
-        <v>1279</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="9" t="s">
+      <c r="I42" s="43"/>
+    </row>
+    <row r="43" spans="1:9">
+      <c r="A43" s="44">
+        <v>4</v>
+      </c>
+      <c r="B43" s="9" t="s">
         <v>1280</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="10" t="s">
+      <c r="C43" s="25"/>
+      <c r="D43" s="39" t="s">
+        <v>1404</v>
+      </c>
+      <c r="E43" t="s">
+        <v>812</v>
+      </c>
+      <c r="I43" s="43"/>
+    </row>
+    <row r="44" spans="1:9">
+      <c r="A44" s="44">
+        <v>77</v>
+      </c>
+      <c r="B44" s="22" t="s">
+        <v>89</v>
+      </c>
+      <c r="C44" s="36"/>
+      <c r="D44" s="37" t="s">
+        <v>1401</v>
+      </c>
+      <c r="E44" s="36" t="s">
+        <v>89</v>
+      </c>
+      <c r="I44" s="43"/>
+    </row>
+    <row r="45" spans="1:9">
+      <c r="A45" s="44">
+        <v>70</v>
+      </c>
+      <c r="B45" s="21" t="s">
+        <v>1331</v>
+      </c>
+      <c r="C45" s="29"/>
+      <c r="D45" s="37" t="s">
+        <v>1401</v>
+      </c>
+      <c r="E45" t="s">
+        <v>1363</v>
+      </c>
+      <c r="I45" s="43"/>
+    </row>
+    <row r="46" spans="1:9">
+      <c r="A46" s="44">
+        <v>74</v>
+      </c>
+      <c r="B46" s="22" t="s">
+        <v>141</v>
+      </c>
+      <c r="C46" s="36"/>
+      <c r="D46" s="37" t="s">
+        <v>1401</v>
+      </c>
+      <c r="E46" s="36" t="s">
+        <v>1378</v>
+      </c>
+      <c r="I46" s="43"/>
+    </row>
+    <row r="47" spans="1:9">
+      <c r="A47" s="44">
+        <v>12</v>
+      </c>
+      <c r="B47" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="C47" s="28"/>
+      <c r="D47" s="44" t="s">
+        <v>1353</v>
+      </c>
+      <c r="E47" s="38" t="s">
+        <v>1340</v>
+      </c>
+      <c r="I47" s="43"/>
+    </row>
+    <row r="48" spans="1:9">
+      <c r="A48" s="44">
+        <v>81</v>
+      </c>
+      <c r="B48" s="22" t="s">
+        <v>1335</v>
+      </c>
+      <c r="C48" s="36"/>
+      <c r="D48" s="37" t="s">
+        <v>1401</v>
+      </c>
+      <c r="E48" s="44" t="s">
+        <v>1390</v>
+      </c>
+      <c r="I48" s="43"/>
+    </row>
+    <row r="49" spans="1:9">
+      <c r="A49" s="44">
+        <v>23</v>
+      </c>
+      <c r="B49" s="17" t="s">
+        <v>1295</v>
+      </c>
+      <c r="C49" s="24"/>
+      <c r="D49" s="44" t="s">
+        <v>1353</v>
+      </c>
+      <c r="E49" s="44" t="s">
+        <v>1353</v>
+      </c>
+      <c r="I49" s="43"/>
+    </row>
+    <row r="50" spans="1:9">
+      <c r="A50" s="44">
         <v>24</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="11" t="s">
-        <v>1281</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="12" t="s">
-        <v>1282</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="13" t="s">
-        <v>1283</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" s="13" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" s="13" t="s">
-        <v>1284</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" s="13" t="s">
-        <v>1285</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="13" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" s="14" t="s">
-        <v>1286</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" s="15" t="s">
-        <v>1287</v>
-      </c>
-      <c r="B15" t="s">
-        <v>1351</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" s="16" t="s">
-        <v>1288</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="16" t="s">
-        <v>1289</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="16" t="s">
-        <v>1290</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="16" t="s">
-        <v>1291</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="16" t="s">
-        <v>1292</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" s="16" t="s">
-        <v>1293</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" s="16" t="s">
-        <v>710</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23" s="16" t="s">
-        <v>1294</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24" s="17" t="s">
-        <v>1295</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
-      <c r="A25" s="18" t="s">
+      <c r="B50" s="18" t="s">
         <v>1296</v>
       </c>
-    </row>
-    <row r="26" spans="1:2">
-      <c r="A26" s="18" t="s">
+      <c r="C50" s="35"/>
+      <c r="D50" s="44" t="s">
+        <v>1431</v>
+      </c>
+      <c r="E50" s="44" t="s">
+        <v>1431</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9">
+      <c r="A51" s="44">
+        <v>25</v>
+      </c>
+      <c r="B51" s="18" t="s">
         <v>1297</v>
       </c>
-    </row>
-    <row r="27" spans="1:2">
-      <c r="A27" s="18" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2">
-      <c r="A28" s="18" t="s">
+      <c r="C51" s="35"/>
+      <c r="D51" s="44" t="s">
+        <v>1431</v>
+      </c>
+      <c r="E51" s="44" t="s">
+        <v>1431</v>
+      </c>
+      <c r="F51" s="44"/>
+      <c r="G51" s="44"/>
+    </row>
+    <row r="52" spans="1:9">
+      <c r="A52" s="44">
+        <v>27</v>
+      </c>
+      <c r="B52" s="18" t="s">
         <v>1298</v>
       </c>
-      <c r="B28" t="s">
-        <v>1352</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2">
-      <c r="A29" s="18" t="s">
+      <c r="C52" s="35"/>
+      <c r="D52" s="44" t="s">
+        <v>1431</v>
+      </c>
+      <c r="E52" s="44" t="s">
+        <v>1431</v>
+      </c>
+      <c r="F52" s="44"/>
+      <c r="G52" s="44"/>
+    </row>
+    <row r="53" spans="1:9">
+      <c r="A53" s="44">
+        <v>28</v>
+      </c>
+      <c r="B53" s="18" t="s">
         <v>1299</v>
       </c>
-    </row>
-    <row r="30" spans="1:2">
-      <c r="A30" s="18" t="s">
-        <v>137</v>
-      </c>
-      <c r="B30" s="18" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2">
-      <c r="A31" s="18" t="s">
-        <v>1300</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2">
-      <c r="A32" s="18" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1">
-      <c r="A33" s="19" t="s">
+      <c r="C53" s="35"/>
+      <c r="D53" s="44" t="s">
+        <v>1431</v>
+      </c>
+      <c r="E53" s="44" t="s">
+        <v>1431</v>
+      </c>
+      <c r="F53" s="44"/>
+      <c r="G53" s="44"/>
+    </row>
+    <row r="54" spans="1:9">
+      <c r="A54" s="44">
+        <v>32</v>
+      </c>
+      <c r="B54" s="19" t="s">
         <v>1301</v>
       </c>
-    </row>
-    <row r="34" spans="1:1">
-      <c r="A34" s="20" t="s">
-        <v>1302</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1">
-      <c r="A35" s="20" t="s">
-        <v>1303</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1">
-      <c r="A36" s="20" t="s">
-        <v>1304</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1">
-      <c r="A37" s="19" t="s">
+      <c r="C54" s="31"/>
+      <c r="D54" s="44" t="s">
+        <v>1431</v>
+      </c>
+      <c r="E54" s="44" t="s">
+        <v>1431</v>
+      </c>
+      <c r="G54" s="44"/>
+      <c r="H54" t="s">
+        <v>1408</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9">
+      <c r="A55" s="44">
+        <v>36</v>
+      </c>
+      <c r="B55" s="19" t="s">
         <v>827</v>
       </c>
-    </row>
-    <row r="38" spans="1:1">
-      <c r="A38" s="19" t="s">
+      <c r="C55" s="38" t="b">
+        <v>1</v>
+      </c>
+      <c r="D55" s="44" t="s">
+        <v>1353</v>
+      </c>
+      <c r="E55" s="44" t="s">
+        <v>1353</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9">
+      <c r="A56" s="44">
+        <v>37</v>
+      </c>
+      <c r="B56" s="19" t="s">
         <v>784</v>
       </c>
-    </row>
-    <row r="39" spans="1:1">
-      <c r="A39" s="20" t="s">
+      <c r="C56" s="38" t="b">
+        <v>1</v>
+      </c>
+      <c r="D56" s="44" t="s">
+        <v>1353</v>
+      </c>
+      <c r="E56" s="44" t="s">
+        <v>1353</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9">
+      <c r="A57" s="44">
+        <v>38</v>
+      </c>
+      <c r="B57" s="20" t="s">
         <v>830</v>
       </c>
-    </row>
-    <row r="40" spans="1:1">
-      <c r="A40" s="20" t="s">
+      <c r="C57" s="32"/>
+      <c r="D57" s="38"/>
+    </row>
+    <row r="58" spans="1:9">
+      <c r="A58" s="44">
+        <v>39</v>
+      </c>
+      <c r="B58" s="20" t="s">
         <v>1305</v>
       </c>
-    </row>
-    <row r="41" spans="1:1">
-      <c r="A41" s="20" t="s">
+      <c r="C58" s="38"/>
+      <c r="D58" s="38"/>
+      <c r="E58" s="44"/>
+    </row>
+    <row r="59" spans="1:9">
+      <c r="A59" s="44">
+        <v>40</v>
+      </c>
+      <c r="B59" s="20" t="s">
         <v>1306</v>
       </c>
-    </row>
-    <row r="42" spans="1:1">
-      <c r="A42" s="20" t="s">
+      <c r="C59" s="32"/>
+      <c r="D59" s="38"/>
+      <c r="E59" s="44"/>
+    </row>
+    <row r="60" spans="1:9">
+      <c r="A60" s="44">
+        <v>41</v>
+      </c>
+      <c r="B60" s="20" t="s">
         <v>1307</v>
       </c>
-    </row>
-    <row r="43" spans="1:1">
-      <c r="A43" s="20" t="s">
+      <c r="C60" s="32"/>
+      <c r="D60" s="38"/>
+      <c r="E60" s="44"/>
+    </row>
+    <row r="61" spans="1:9">
+      <c r="A61" s="44">
+        <v>42</v>
+      </c>
+      <c r="B61" s="20" t="s">
         <v>1308</v>
       </c>
-    </row>
-    <row r="44" spans="1:1">
-      <c r="A44" s="20" t="s">
+      <c r="C61" s="32"/>
+      <c r="D61" s="38"/>
+      <c r="E61" s="44"/>
+    </row>
+    <row r="62" spans="1:9">
+      <c r="A62" s="44">
+        <v>43</v>
+      </c>
+      <c r="B62" s="20" t="s">
         <v>828</v>
       </c>
-    </row>
-    <row r="45" spans="1:1">
-      <c r="A45" s="20" t="s">
+      <c r="C62" s="32"/>
+      <c r="D62" s="38"/>
+      <c r="E62" s="44"/>
+    </row>
+    <row r="63" spans="1:9">
+      <c r="A63" s="44">
+        <v>44</v>
+      </c>
+      <c r="B63" s="20" t="s">
         <v>1309</v>
       </c>
-    </row>
-    <row r="46" spans="1:1">
-      <c r="A46" s="20" t="s">
+      <c r="C63" s="38" t="b">
+        <v>1</v>
+      </c>
+      <c r="D63" s="44" t="s">
+        <v>1353</v>
+      </c>
+      <c r="E63" s="44" t="s">
+        <v>1353</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9">
+      <c r="A64" s="44">
+        <v>45</v>
+      </c>
+      <c r="B64" s="20" t="s">
         <v>715</v>
       </c>
-    </row>
-    <row r="47" spans="1:1">
-      <c r="A47" s="19" t="s">
+      <c r="C64" s="38" t="b">
+        <v>1</v>
+      </c>
+      <c r="D64" s="44" t="s">
+        <v>1353</v>
+      </c>
+      <c r="E64" s="44" t="s">
+        <v>1353</v>
+      </c>
+      <c r="F64" s="44"/>
+      <c r="G64" s="44"/>
+    </row>
+    <row r="65" spans="1:7">
+      <c r="A65" s="44">
+        <v>46</v>
+      </c>
+      <c r="B65" s="18" t="s">
         <v>1310</v>
       </c>
-    </row>
-    <row r="48" spans="1:1">
-      <c r="A48" s="20" t="s">
-        <v>1311</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1">
-      <c r="A49" s="20" t="s">
+      <c r="C65" s="35"/>
+      <c r="D65" s="38"/>
+      <c r="F65" s="44"/>
+      <c r="G65" s="44"/>
+    </row>
+    <row r="66" spans="1:7">
+      <c r="A66" s="44">
+        <v>48</v>
+      </c>
+      <c r="B66" s="18" t="s">
         <v>1312</v>
       </c>
-    </row>
-    <row r="50" spans="1:1">
-      <c r="A50" s="20" t="s">
+      <c r="C66" s="35"/>
+      <c r="D66" s="38"/>
+      <c r="F66" s="44"/>
+      <c r="G66" s="44"/>
+    </row>
+    <row r="67" spans="1:7">
+      <c r="A67" s="44">
+        <v>49</v>
+      </c>
+      <c r="B67" s="18" t="s">
         <v>1313</v>
       </c>
-    </row>
-    <row r="51" spans="1:1">
-      <c r="A51" s="19" t="s">
+      <c r="C67" s="35"/>
+      <c r="D67" s="38"/>
+      <c r="E67" s="44"/>
+    </row>
+    <row r="68" spans="1:7">
+      <c r="A68" s="44">
+        <v>50</v>
+      </c>
+      <c r="B68" s="18" t="s">
         <v>1314</v>
       </c>
-    </row>
-    <row r="52" spans="1:1">
-      <c r="A52" s="18" t="s">
+      <c r="C68" s="35"/>
+      <c r="D68" s="38"/>
+      <c r="E68" s="44"/>
+      <c r="F68" t="s">
+        <v>1422</v>
+      </c>
+      <c r="G68" t="s">
+        <v>1423</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7">
+      <c r="A69" s="44">
+        <v>51</v>
+      </c>
+      <c r="B69" s="18" t="s">
         <v>1315</v>
       </c>
-    </row>
-    <row r="53" spans="1:1">
-      <c r="A53" s="18" t="s">
+      <c r="C69" s="35"/>
+      <c r="D69" s="38"/>
+      <c r="E69" s="44"/>
+      <c r="F69" t="s">
+        <v>1425</v>
+      </c>
+      <c r="G69" t="s">
+        <v>1423</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7">
+      <c r="A70" s="44">
+        <v>52</v>
+      </c>
+      <c r="B70" s="20" t="s">
         <v>1316</v>
       </c>
-    </row>
-    <row r="54" spans="1:1">
-      <c r="A54" s="18" t="s">
+      <c r="C70" s="32"/>
+      <c r="D70" s="38"/>
+      <c r="F70" t="s">
+        <v>1429</v>
+      </c>
+      <c r="G70" t="s">
+        <v>1423</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7">
+      <c r="A71" s="44">
+        <v>53</v>
+      </c>
+      <c r="B71" s="20" t="s">
         <v>1317</v>
       </c>
-    </row>
-    <row r="55" spans="1:1">
-      <c r="A55" s="18" t="s">
+      <c r="C71" s="32"/>
+      <c r="D71" s="38"/>
+      <c r="F71" t="s">
+        <v>1424</v>
+      </c>
+      <c r="G71" t="s">
+        <v>1423</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7">
+      <c r="A72" s="44">
+        <v>54</v>
+      </c>
+      <c r="B72" s="20" t="s">
         <v>1318</v>
       </c>
-    </row>
-    <row r="56" spans="1:1">
-      <c r="A56" s="18" t="s">
+      <c r="C72" s="32"/>
+      <c r="D72" s="38"/>
+      <c r="E72" s="44"/>
+    </row>
+    <row r="73" spans="1:7">
+      <c r="A73" s="44">
+        <v>55</v>
+      </c>
+      <c r="B73" s="20" t="s">
         <v>1319</v>
       </c>
-    </row>
-    <row r="57" spans="1:1">
-      <c r="A57" s="18" t="s">
+      <c r="C73" s="32"/>
+      <c r="D73" s="38"/>
+    </row>
+    <row r="74" spans="1:7">
+      <c r="A74" s="44">
+        <v>56</v>
+      </c>
+      <c r="B74" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="C74" s="32"/>
+      <c r="D74" s="38"/>
+      <c r="F74" t="s">
+        <v>1421</v>
+      </c>
+      <c r="G74" t="s">
+        <v>1420</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7">
+      <c r="A75" s="44">
+        <v>57</v>
+      </c>
+      <c r="B75" s="20" t="s">
         <v>1320</v>
       </c>
-    </row>
-    <row r="58" spans="1:1">
-      <c r="A58" s="20" t="s">
+      <c r="C75" s="32"/>
+      <c r="D75" s="38"/>
+      <c r="E75" s="40"/>
+    </row>
+    <row r="76" spans="1:7">
+      <c r="A76" s="44">
+        <v>58</v>
+      </c>
+      <c r="B76" s="20" t="s">
         <v>1321</v>
       </c>
-    </row>
-    <row r="59" spans="1:1">
-      <c r="A59" s="20" t="s">
+      <c r="C76" s="32"/>
+      <c r="D76" s="38"/>
+      <c r="E76" s="40"/>
+    </row>
+    <row r="77" spans="1:7">
+      <c r="A77" s="44">
+        <v>59</v>
+      </c>
+      <c r="B77" s="18" t="s">
         <v>1322</v>
       </c>
-    </row>
-    <row r="60" spans="1:1">
-      <c r="A60" s="20" t="s">
+      <c r="C77" s="35"/>
+      <c r="D77" s="38"/>
+      <c r="E77" s="40"/>
+      <c r="F77" t="s">
+        <v>1419</v>
+      </c>
+      <c r="G77" t="s">
+        <v>1418</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7">
+      <c r="A78" s="44">
+        <v>60</v>
+      </c>
+      <c r="B78" s="18" t="s">
         <v>1323</v>
       </c>
-    </row>
-    <row r="61" spans="1:1">
-      <c r="A61" s="20" t="s">
+      <c r="C78" s="35"/>
+      <c r="D78" s="38"/>
+      <c r="E78" s="40"/>
+    </row>
+    <row r="79" spans="1:7">
+      <c r="A79" s="44">
+        <v>61</v>
+      </c>
+      <c r="B79" s="18" t="s">
         <v>1324</v>
       </c>
-    </row>
-    <row r="62" spans="1:1">
-      <c r="A62" s="20" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="63" spans="1:1">
-      <c r="A63" s="20" t="s">
+      <c r="C79" s="35"/>
+      <c r="D79" s="38"/>
+      <c r="E79" s="40"/>
+    </row>
+    <row r="80" spans="1:7">
+      <c r="A80" s="44">
+        <v>62</v>
+      </c>
+      <c r="B80" s="20" t="s">
+        <v>867</v>
+      </c>
+      <c r="C80" s="32"/>
+      <c r="D80" s="38"/>
+      <c r="E80" s="43"/>
+    </row>
+    <row r="81" spans="1:8">
+      <c r="A81" s="44">
+        <v>63</v>
+      </c>
+      <c r="B81" s="20" t="s">
+        <v>886</v>
+      </c>
+      <c r="C81" s="32"/>
+      <c r="D81" s="38"/>
+      <c r="F81" t="s">
+        <v>1428</v>
+      </c>
+      <c r="G81" t="s">
+        <v>1423</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8">
+      <c r="A82" s="44">
+        <v>64</v>
+      </c>
+      <c r="B82" s="20" t="s">
         <v>1325</v>
       </c>
-    </row>
-    <row r="64" spans="1:1">
-      <c r="A64" s="20" t="s">
+      <c r="C82" s="32"/>
+      <c r="D82" s="38"/>
+      <c r="F82" t="s">
+        <v>1426</v>
+      </c>
+      <c r="G82" t="s">
+        <v>1423</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8">
+      <c r="A83" s="44">
+        <v>65</v>
+      </c>
+      <c r="B83" s="20" t="s">
         <v>1326</v>
       </c>
-    </row>
-    <row r="65" spans="1:1">
-      <c r="A65" s="18" t="s">
-        <v>1327</v>
-      </c>
-    </row>
-    <row r="66" spans="1:1">
-      <c r="A66" s="18" t="s">
-        <v>1328</v>
-      </c>
-    </row>
-    <row r="67" spans="1:1">
-      <c r="A67" s="18" t="s">
-        <v>1329</v>
-      </c>
-    </row>
-    <row r="68" spans="1:1">
-      <c r="A68" s="20" t="s">
-        <v>867</v>
-      </c>
-    </row>
-    <row r="69" spans="1:1">
-      <c r="A69" s="20" t="s">
-        <v>886</v>
-      </c>
-    </row>
-    <row r="70" spans="1:1">
-      <c r="A70" s="20" t="s">
-        <v>1330</v>
-      </c>
-    </row>
-    <row r="71" spans="1:1">
-      <c r="A71" s="20" t="s">
-        <v>1331</v>
-      </c>
-    </row>
-    <row r="72" spans="1:1">
-      <c r="A72" s="20" t="s">
-        <v>1332</v>
-      </c>
-    </row>
-    <row r="73" spans="1:1">
-      <c r="A73" s="18" t="s">
+      <c r="C83" s="32"/>
+      <c r="D83" s="38"/>
+      <c r="F83" t="s">
+        <v>1427</v>
+      </c>
+      <c r="G83" t="s">
+        <v>1423</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8">
+      <c r="A84" s="44">
+        <v>72</v>
+      </c>
+      <c r="B84" s="22" t="s">
         <v>1333</v>
       </c>
-    </row>
-    <row r="74" spans="1:1">
-      <c r="A74" s="18" t="s">
+      <c r="C84" s="36"/>
+      <c r="D84" s="38"/>
+      <c r="E84" s="44"/>
+    </row>
+    <row r="85" spans="1:8">
+      <c r="A85" s="44">
+        <v>80</v>
+      </c>
+      <c r="B85" s="22" t="s">
         <v>1334</v>
       </c>
-    </row>
-    <row r="75" spans="1:1">
-      <c r="A75" s="18" t="s">
-        <v>1335</v>
-      </c>
-    </row>
-    <row r="76" spans="1:1">
-      <c r="A76" s="21" t="s">
-        <v>1336</v>
-      </c>
-    </row>
-    <row r="77" spans="1:1">
-      <c r="A77" s="21" t="s">
-        <v>1337</v>
-      </c>
-    </row>
-    <row r="78" spans="1:1">
-      <c r="A78" s="22" t="s">
-        <v>1338</v>
-      </c>
-    </row>
-    <row r="79" spans="1:1">
-      <c r="A79" s="22" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="80" spans="1:1">
-      <c r="A80" s="22" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="81" spans="1:1">
-      <c r="A81" s="22" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="82" spans="1:1">
-      <c r="A82" s="22" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="83" spans="1:1">
-      <c r="A83" s="22" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="84" spans="1:1">
-      <c r="A84" s="22" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="85" spans="1:1">
-      <c r="A85" s="22" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="86" spans="1:1">
-      <c r="A86" s="22" t="s">
+      <c r="C85" s="36"/>
+      <c r="D85" s="38"/>
+    </row>
+    <row r="86" spans="1:8">
+      <c r="A86" s="44">
+        <v>85</v>
+      </c>
+      <c r="B86" s="22" t="s">
         <v>1339</v>
       </c>
-    </row>
-    <row r="87" spans="1:1">
-      <c r="A87" s="22" t="s">
-        <v>1340</v>
-      </c>
-    </row>
-    <row r="88" spans="1:1">
-      <c r="A88" s="22" t="s">
-        <v>1341</v>
-      </c>
-    </row>
-    <row r="89" spans="1:1">
-      <c r="A89" s="22" t="s">
-        <v>1342</v>
-      </c>
-    </row>
-    <row r="90" spans="1:1">
-      <c r="A90" s="22" t="s">
-        <v>1343</v>
-      </c>
-    </row>
-    <row r="91" spans="1:1">
-      <c r="A91" s="22" t="s">
-        <v>1344</v>
-      </c>
-    </row>
-    <row r="92" spans="1:1">
-      <c r="A92" s="23" t="s">
-        <v>1345</v>
-      </c>
-    </row>
-    <row r="93" spans="1:1">
-      <c r="A93" s="23" t="s">
-        <v>1346</v>
-      </c>
-    </row>
-    <row r="94" spans="1:1">
-      <c r="A94" s="23" t="s">
-        <v>1347</v>
-      </c>
-    </row>
-    <row r="95" spans="1:1">
-      <c r="A95" s="23" t="s">
-        <v>1348</v>
-      </c>
-    </row>
-    <row r="96" spans="1:1">
-      <c r="A96" s="23" t="s">
-        <v>1349</v>
-      </c>
-    </row>
-    <row r="97" spans="1:1">
-      <c r="A97" s="24" t="s">
-        <v>1350</v>
+      <c r="C86" s="36"/>
+      <c r="D86" s="38"/>
+      <c r="F86" t="s">
+        <v>1411</v>
+      </c>
+      <c r="G86" t="s">
+        <v>1410</v>
+      </c>
+      <c r="H86" t="s">
+        <v>1410</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A77:A79 A1">
-    <cfRule type="cellIs" dxfId="10" priority="5" operator="equal">
+  <autoFilter ref="A1:G86" xr:uid="{5E5F9EF8-3CBA-4CCB-8F7D-668C099D13C0}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G86">
+      <sortCondition ref="E1:E86"/>
+    </sortState>
+  </autoFilter>
+  <conditionalFormatting sqref="B1:D1 D74:D79 B73:D74 B72:C72">
+    <cfRule type="cellIs" dxfId="108" priority="103" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:A97">
-    <cfRule type="cellIs" dxfId="9" priority="6" operator="equal">
+  <conditionalFormatting sqref="B1:D1 B16:D17 B13:D13 B15:C15 B2:C5 B22:D39 B14 B6:B12 B18:B21 D18:D20 B40 D40 B48 B67 B68:D71 B73:D79 B72:C72 B81:D82 B80:C80 B84:D84 B83:C83 B86:D86 B85:C85 B41:D47 B57:D62 B49:E56 B65:D66 B63:E64">
+    <cfRule type="cellIs" dxfId="107" priority="104" operator="equal">
       <formula>"FALSE - definition only"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="106" priority="105" operator="equal">
       <formula>"-"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="9" operator="containsText" text="NULL">
-      <formula>NOT(ISERROR(SEARCH(("NULL"),(A1))))</formula>
+    <cfRule type="containsText" dxfId="105" priority="107" operator="containsText" text="NULL">
+      <formula>NOT(ISERROR(SEARCH(("NULL"),(B1))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A23:A24 A26">
-    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
+  <conditionalFormatting sqref="B23:D24 B26:D26">
+    <cfRule type="cellIs" dxfId="104" priority="102" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A77:A79">
-    <cfRule type="cellIs" dxfId="5" priority="8" operator="equal">
+  <conditionalFormatting sqref="D74:D79 B73:D74 B72:C72">
+    <cfRule type="cellIs" dxfId="103" priority="106" operator="equal">
+      <formula>""""""</formula>
+    </cfRule>
+    <cfRule type="containsBlanks" dxfId="102" priority="108">
+      <formula>LEN(TRIM(#REF!))=0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="101" priority="109" operator="equal">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A77:A79">
-    <cfRule type="containsBlanks" dxfId="4" priority="10">
+  <conditionalFormatting sqref="E30">
+    <cfRule type="cellIs" dxfId="100" priority="99" operator="equal">
+      <formula>"FALSE - definition only"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="99" priority="100" operator="equal">
+      <formula>"-"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="98" priority="101" operator="containsText" text="NULL">
+      <formula>NOT(ISERROR(SEARCH(("NULL"),(E30))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E3:E4">
+    <cfRule type="cellIs" dxfId="97" priority="96" operator="equal">
+      <formula>"FALSE - definition only"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="96" priority="97" operator="equal">
+      <formula>"-"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="95" priority="98" operator="containsText" text="NULL">
+      <formula>NOT(ISERROR(SEARCH(("NULL"),(E3))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E6:E14">
+    <cfRule type="cellIs" dxfId="94" priority="93" operator="equal">
+      <formula>"FALSE - definition only"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="93" priority="94" operator="equal">
+      <formula>"-"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="92" priority="95" operator="containsText" text="NULL">
+      <formula>NOT(ISERROR(SEARCH(("NULL"),(E6))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D18:E20">
+    <cfRule type="cellIs" dxfId="91" priority="90" operator="equal">
+      <formula>"FALSE - definition only"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="90" priority="91" operator="equal">
+      <formula>"-"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="89" priority="92" operator="containsText" text="NULL">
+      <formula>NOT(ISERROR(SEARCH(("NULL"),(D18))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E79">
+    <cfRule type="cellIs" dxfId="88" priority="87" operator="equal">
+      <formula>"FALSE - definition only"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="87" priority="88" operator="equal">
+      <formula>"-"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="86" priority="89" operator="containsText" text="NULL">
+      <formula>NOT(ISERROR(SEARCH(("NULL"),(E79))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E77:E78">
+    <cfRule type="cellIs" dxfId="85" priority="84" operator="equal">
+      <formula>"FALSE - definition only"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="84" priority="85" operator="equal">
+      <formula>"-"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="83" priority="86" operator="containsText" text="NULL">
+      <formula>NOT(ISERROR(SEARCH(("NULL"),(E77))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E21">
+    <cfRule type="cellIs" dxfId="82" priority="81" operator="equal">
+      <formula>"FALSE - definition only"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="81" priority="82" operator="equal">
+      <formula>"-"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="80" priority="83" operator="containsText" text="NULL">
+      <formula>NOT(ISERROR(SEARCH(("NULL"),(E21))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D21">
+    <cfRule type="cellIs" dxfId="79" priority="78" operator="equal">
+      <formula>"FALSE - definition only"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="78" priority="79" operator="equal">
+      <formula>"-"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="77" priority="80" operator="containsText" text="NULL">
+      <formula>NOT(ISERROR(SEARCH(("NULL"),(D21))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D12 D6:D8">
+    <cfRule type="cellIs" dxfId="76" priority="75" operator="equal">
+      <formula>"FALSE - definition only"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="75" priority="76" operator="equal">
+      <formula>"-"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="74" priority="77" operator="containsText" text="NULL">
+      <formula>NOT(ISERROR(SEARCH(("NULL"),(D6))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D14">
+    <cfRule type="cellIs" dxfId="73" priority="72" operator="equal">
+      <formula>"FALSE - definition only"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="72" priority="73" operator="equal">
+      <formula>"-"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="71" priority="74" operator="containsText" text="NULL">
+      <formula>NOT(ISERROR(SEARCH(("NULL"),(D14))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D3:D4">
+    <cfRule type="cellIs" dxfId="70" priority="69" operator="equal">
+      <formula>"FALSE - definition only"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="69" priority="70" operator="equal">
+      <formula>"-"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="68" priority="71" operator="containsText" text="NULL">
+      <formula>NOT(ISERROR(SEARCH(("NULL"),(D3))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G22:H22">
+    <cfRule type="cellIs" dxfId="67" priority="66" operator="equal">
+      <formula>"FALSE - definition only"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="66" priority="67" operator="equal">
+      <formula>"-"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="65" priority="68" operator="containsText" text="NULL">
+      <formula>NOT(ISERROR(SEARCH(("NULL"),(G22))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C12">
+    <cfRule type="cellIs" dxfId="64" priority="63" operator="equal">
+      <formula>"FALSE - definition only"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="63" priority="64" operator="equal">
+      <formula>"-"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="62" priority="65" operator="containsText" text="NULL">
+      <formula>NOT(ISERROR(SEARCH(("NULL"),(C12))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C18:C21">
+    <cfRule type="cellIs" dxfId="61" priority="60" operator="equal">
+      <formula>"FALSE - definition only"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="60" priority="61" operator="equal">
+      <formula>"-"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="59" priority="62" operator="containsText" text="NULL">
+      <formula>NOT(ISERROR(SEARCH(("NULL"),(C18))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C14">
+    <cfRule type="cellIs" dxfId="58" priority="57" operator="equal">
+      <formula>"FALSE - definition only"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="57" priority="58" operator="equal">
+      <formula>"-"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="56" priority="59" operator="containsText" text="NULL">
+      <formula>NOT(ISERROR(SEARCH(("NULL"),(C14))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C11">
+    <cfRule type="cellIs" dxfId="55" priority="54" operator="equal">
+      <formula>"FALSE - definition only"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="54" priority="55" operator="equal">
+      <formula>"-"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="53" priority="56" operator="containsText" text="NULL">
+      <formula>NOT(ISERROR(SEARCH(("NULL"),(C11))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C10">
+    <cfRule type="cellIs" dxfId="52" priority="51" operator="equal">
+      <formula>"FALSE - definition only"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="51" priority="52" operator="equal">
+      <formula>"-"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="50" priority="53" operator="containsText" text="NULL">
+      <formula>NOT(ISERROR(SEARCH(("NULL"),(C10))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C9">
+    <cfRule type="cellIs" dxfId="49" priority="48" operator="equal">
+      <formula>"FALSE - definition only"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="48" priority="49" operator="equal">
+      <formula>"-"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="47" priority="50" operator="containsText" text="NULL">
+      <formula>NOT(ISERROR(SEARCH(("NULL"),(C9))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C8">
+    <cfRule type="cellIs" dxfId="46" priority="45" operator="equal">
+      <formula>"FALSE - definition only"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="45" priority="46" operator="equal">
+      <formula>"-"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="44" priority="47" operator="containsText" text="NULL">
+      <formula>NOT(ISERROR(SEARCH(("NULL"),(C8))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C7">
+    <cfRule type="cellIs" dxfId="43" priority="42" operator="equal">
+      <formula>"FALSE - definition only"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="42" priority="43" operator="equal">
+      <formula>"-"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="41" priority="44" operator="containsText" text="NULL">
+      <formula>NOT(ISERROR(SEARCH(("NULL"),(C7))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C6">
+    <cfRule type="cellIs" dxfId="40" priority="39" operator="equal">
+      <formula>"FALSE - definition only"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="39" priority="40" operator="equal">
+      <formula>"-"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="38" priority="41" operator="containsText" text="NULL">
+      <formula>NOT(ISERROR(SEARCH(("NULL"),(C6))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C40">
+    <cfRule type="cellIs" dxfId="37" priority="36" operator="equal">
+      <formula>"FALSE - definition only"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="36" priority="37" operator="equal">
+      <formula>"-"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="35" priority="38" operator="containsText" text="NULL">
+      <formula>NOT(ISERROR(SEARCH(("NULL"),(C40))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E48">
+    <cfRule type="cellIs" dxfId="34" priority="33" operator="equal">
+      <formula>"FALSE - definition only"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="33" priority="34" operator="equal">
+      <formula>"-"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="32" priority="35" operator="containsText" text="NULL">
+      <formula>NOT(ISERROR(SEARCH(("NULL"),(E48))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C48">
+    <cfRule type="cellIs" dxfId="31" priority="30" operator="equal">
+      <formula>"FALSE - definition only"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="30" priority="31" operator="equal">
+      <formula>"-"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="29" priority="32" operator="containsText" text="NULL">
+      <formula>NOT(ISERROR(SEARCH(("NULL"),(C48))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E76">
+    <cfRule type="cellIs" dxfId="28" priority="27" operator="equal">
+      <formula>"FALSE - definition only"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="27" priority="28" operator="equal">
+      <formula>"-"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="26" priority="29" operator="containsText" text="NULL">
+      <formula>NOT(ISERROR(SEARCH(("NULL"),(E76))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E75">
+    <cfRule type="cellIs" dxfId="25" priority="24" operator="equal">
+      <formula>"FALSE - definition only"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="24" priority="25" operator="equal">
+      <formula>"-"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="23" priority="26" operator="containsText" text="NULL">
+      <formula>NOT(ISERROR(SEARCH(("NULL"),(E75))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D82">
+    <cfRule type="cellIs" dxfId="22" priority="20" operator="equal">
+      <formula>"-"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D82">
+    <cfRule type="cellIs" dxfId="21" priority="21" operator="equal">
+      <formula>""""""</formula>
+    </cfRule>
+    <cfRule type="containsBlanks" dxfId="20" priority="22">
       <formula>LEN(TRIM(#REF!))=0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="23" operator="equal">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B30">
+  <conditionalFormatting sqref="C67">
+    <cfRule type="cellIs" dxfId="18" priority="17" operator="equal">
+      <formula>"FALSE - definition only"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="17" priority="18" operator="equal">
+      <formula>"-"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="16" priority="19" operator="containsText" text="NULL">
+      <formula>NOT(ISERROR(SEARCH(("NULL"),(C67))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D71">
+    <cfRule type="cellIs" dxfId="15" priority="13" operator="equal">
+      <formula>"-"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D71">
+    <cfRule type="cellIs" dxfId="14" priority="14" operator="equal">
+      <formula>""""""</formula>
+    </cfRule>
+    <cfRule type="containsBlanks" dxfId="13" priority="15">
+      <formula>LEN(TRIM(#REF!))=0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="16" operator="equal">
+      <formula>""""""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D48">
+    <cfRule type="cellIs" dxfId="11" priority="10" operator="equal">
+      <formula>"FALSE - definition only"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
+      <formula>"-"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="9" priority="12" operator="containsText" text="NULL">
+      <formula>NOT(ISERROR(SEARCH(("NULL"),(D48))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D11">
+    <cfRule type="cellIs" dxfId="8" priority="7" operator="equal">
+      <formula>"FALSE - definition only"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
+      <formula>"-"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="9" operator="containsText" text="NULL">
+      <formula>NOT(ISERROR(SEARCH(("NULL"),(D11))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D10">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
+      <formula>"FALSE - definition only"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+      <formula>"-"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="NULL">
+      <formula>NOT(ISERROR(SEARCH(("NULL"),(D10))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D9">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"FALSE - definition only"</formula>
     </cfRule>
@@ -15440,20 +18139,458 @@
       <formula>"-"</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="NULL">
-      <formula>NOT(ISERROR(SEARCH(("NULL"),(B30))))</formula>
+      <formula>NOT(ISERROR(SEARCH(("NULL"),(D9))))</formula>
     </cfRule>
   </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54536A3A-BDBB-415D-84AF-C51CC211CC9A}">
+  <dimension ref="A1:AN36"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
+    </sheetView>
+    <sheetView workbookViewId="1">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="34.42578125" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.28515625" customWidth="1"/>
+    <col min="4" max="4" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="34.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:40">
+      <c r="A1" s="39" t="s">
+        <v>1404</v>
+      </c>
+      <c r="B1" s="39" t="s">
+        <v>1403</v>
+      </c>
+      <c r="C1" s="39" t="s">
+        <v>1402</v>
+      </c>
+      <c r="D1" s="37" t="s">
+        <v>1400</v>
+      </c>
+      <c r="E1" s="37" t="s">
+        <v>1401</v>
+      </c>
+    </row>
+    <row r="2" spans="1:40">
+      <c r="A2" s="44" t="s">
+        <v>1354</v>
+      </c>
+      <c r="B2" s="43" t="s">
+        <v>1354</v>
+      </c>
+      <c r="C2" s="44" t="s">
+        <v>1342</v>
+      </c>
+      <c r="D2" s="43" t="s">
+        <v>1342</v>
+      </c>
+      <c r="E2" s="44" t="s">
+        <v>1342</v>
+      </c>
+    </row>
+    <row r="3" spans="1:40">
+      <c r="A3" s="44" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="43" t="s">
+        <v>1341</v>
+      </c>
+      <c r="C3" s="44" t="s">
+        <v>1341</v>
+      </c>
+      <c r="D3" s="43" t="s">
+        <v>1341</v>
+      </c>
+      <c r="E3" s="44" t="s">
+        <v>1341</v>
+      </c>
+      <c r="F3" s="44"/>
+      <c r="G3" s="44"/>
+      <c r="H3" s="44"/>
+      <c r="I3" s="44"/>
+      <c r="J3" s="44"/>
+      <c r="K3" s="44"/>
+      <c r="L3" s="44"/>
+      <c r="M3" s="44"/>
+      <c r="N3" s="44"/>
+      <c r="O3" s="44"/>
+      <c r="P3" s="44"/>
+      <c r="Q3" s="44"/>
+      <c r="R3" s="44"/>
+      <c r="S3" s="44"/>
+      <c r="T3" s="44"/>
+      <c r="U3" s="44"/>
+      <c r="V3" s="44"/>
+      <c r="W3" s="44"/>
+      <c r="X3" s="44"/>
+      <c r="Y3" s="44"/>
+      <c r="Z3" s="44"/>
+      <c r="AA3" s="44"/>
+      <c r="AB3" s="44"/>
+      <c r="AC3" s="44"/>
+      <c r="AD3" s="44"/>
+      <c r="AE3" s="44"/>
+      <c r="AF3" s="44"/>
+      <c r="AG3" s="44"/>
+      <c r="AH3" s="44"/>
+      <c r="AI3" s="44"/>
+      <c r="AJ3" s="44"/>
+      <c r="AK3" s="44"/>
+      <c r="AL3" s="44"/>
+      <c r="AM3" s="44"/>
+      <c r="AN3" s="44"/>
+    </row>
+    <row r="4" spans="1:40">
+      <c r="A4" s="44" t="s">
+        <v>1342</v>
+      </c>
+      <c r="B4" s="43" t="s">
+        <v>1343</v>
+      </c>
+      <c r="C4" s="44" t="s">
+        <v>1343</v>
+      </c>
+      <c r="D4" s="43" t="s">
+        <v>1343</v>
+      </c>
+      <c r="E4" s="44" t="s">
+        <v>1343</v>
+      </c>
+    </row>
+    <row r="5" spans="1:40">
+      <c r="A5" s="44" t="s">
+        <v>1394</v>
+      </c>
+      <c r="B5" s="43" t="s">
+        <v>1355</v>
+      </c>
+      <c r="C5" s="44" t="s">
+        <v>1344</v>
+      </c>
+      <c r="D5" s="43" t="s">
+        <v>1361</v>
+      </c>
+      <c r="E5" s="44" t="s">
+        <v>1356</v>
+      </c>
+    </row>
+    <row r="6" spans="1:40">
+      <c r="A6" s="44" t="s">
+        <v>812</v>
+      </c>
+      <c r="B6" s="43" t="s">
+        <v>1356</v>
+      </c>
+      <c r="C6" s="44" t="s">
+        <v>1345</v>
+      </c>
+      <c r="D6" s="43" t="s">
+        <v>1362</v>
+      </c>
+      <c r="E6" s="44" t="s">
+        <v>1357</v>
+      </c>
+    </row>
+    <row r="7" spans="1:40">
+      <c r="A7" s="44" t="s">
+        <v>1395</v>
+      </c>
+      <c r="B7" s="43" t="s">
+        <v>1357</v>
+      </c>
+      <c r="C7" s="44" t="s">
+        <v>1346</v>
+      </c>
+      <c r="D7" s="43" t="s">
+        <v>1363</v>
+      </c>
+      <c r="E7" s="44" t="s">
+        <v>1355</v>
+      </c>
+    </row>
+    <row r="8" spans="1:40">
+      <c r="B8" s="43" t="s">
+        <v>1358</v>
+      </c>
+      <c r="C8" s="44" t="s">
+        <v>1347</v>
+      </c>
+      <c r="D8" s="43" t="s">
+        <v>1344</v>
+      </c>
+      <c r="E8" s="44" t="s">
+        <v>1346</v>
+      </c>
+    </row>
+    <row r="9" spans="1:40">
+      <c r="B9" s="43" t="s">
+        <v>1359</v>
+      </c>
+      <c r="C9" s="44" t="s">
+        <v>1348</v>
+      </c>
+      <c r="D9" s="43" t="s">
+        <v>1345</v>
+      </c>
+      <c r="E9" s="44" t="s">
+        <v>1361</v>
+      </c>
+    </row>
+    <row r="10" spans="1:40">
+      <c r="B10" s="43" t="s">
+        <v>1360</v>
+      </c>
+      <c r="C10" s="44" t="s">
+        <v>1349</v>
+      </c>
+      <c r="D10" s="43" t="s">
+        <v>1346</v>
+      </c>
+      <c r="E10" s="44" t="s">
+        <v>1362</v>
+      </c>
+    </row>
+    <row r="11" spans="1:40">
+      <c r="B11" s="43"/>
+      <c r="C11" s="44" t="s">
+        <v>1350</v>
+      </c>
+      <c r="D11" s="43" t="s">
+        <v>1364</v>
+      </c>
+      <c r="E11" s="44" t="s">
+        <v>1351</v>
+      </c>
+    </row>
+    <row r="12" spans="1:40">
+      <c r="B12" s="43"/>
+      <c r="C12" s="44" t="s">
+        <v>132</v>
+      </c>
+      <c r="D12" s="43" t="s">
+        <v>1365</v>
+      </c>
+      <c r="E12" s="44" t="s">
+        <v>1367</v>
+      </c>
+    </row>
+    <row r="13" spans="1:40">
+      <c r="B13" s="43"/>
+      <c r="C13" s="44" t="s">
+        <v>768</v>
+      </c>
+      <c r="D13" s="43" t="s">
+        <v>1366</v>
+      </c>
+      <c r="E13" s="44" t="s">
+        <v>1368</v>
+      </c>
+    </row>
+    <row r="14" spans="1:40">
+      <c r="B14" s="43"/>
+      <c r="C14" s="44" t="s">
+        <v>1351</v>
+      </c>
+      <c r="D14" s="43" t="s">
+        <v>1351</v>
+      </c>
+      <c r="E14" s="44" t="s">
+        <v>1369</v>
+      </c>
+    </row>
+    <row r="15" spans="1:40">
+      <c r="B15" s="43"/>
+      <c r="C15" s="44" t="s">
+        <v>1352</v>
+      </c>
+      <c r="D15" s="43" t="s">
+        <v>1367</v>
+      </c>
+      <c r="E15" s="44" t="s">
+        <v>1370</v>
+      </c>
+    </row>
+    <row r="16" spans="1:40">
+      <c r="B16" s="43"/>
+      <c r="C16" s="43"/>
+      <c r="D16" s="43" t="s">
+        <v>1368</v>
+      </c>
+      <c r="E16" s="44" t="s">
+        <v>1377</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5">
+      <c r="B17" s="43"/>
+      <c r="C17" s="43"/>
+      <c r="D17" s="43" t="s">
+        <v>1369</v>
+      </c>
+      <c r="E17" s="44" t="s">
+        <v>1378</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5">
+      <c r="B18" s="43"/>
+      <c r="C18" s="43"/>
+      <c r="D18" s="43" t="s">
+        <v>1370</v>
+      </c>
+      <c r="E18" s="44" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5">
+      <c r="B19" s="43"/>
+      <c r="C19" s="43"/>
+      <c r="D19" s="43" t="s">
+        <v>1371</v>
+      </c>
+      <c r="E19" s="44" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5">
+      <c r="B20" s="43"/>
+      <c r="C20" s="43"/>
+      <c r="D20" s="43" t="s">
+        <v>1372</v>
+      </c>
+      <c r="E20" s="44" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5">
+      <c r="B21" s="43"/>
+      <c r="C21" s="43"/>
+      <c r="D21" s="43" t="s">
+        <v>771</v>
+      </c>
+      <c r="E21" s="44" t="s">
+        <v>1379</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5">
+      <c r="B22" s="43"/>
+      <c r="C22" s="43"/>
+      <c r="D22" s="43" t="s">
+        <v>1373</v>
+      </c>
+      <c r="E22" s="44" t="s">
+        <v>1380</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5">
+      <c r="B23" s="43"/>
+      <c r="C23" s="43"/>
+      <c r="D23" s="43" t="s">
+        <v>1374</v>
+      </c>
+      <c r="E23" s="44" t="s">
+        <v>1381</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5">
+      <c r="B24" s="43"/>
+      <c r="C24" s="43"/>
+      <c r="D24" s="43" t="s">
+        <v>1375</v>
+      </c>
+      <c r="E24" s="44" t="s">
+        <v>1382</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5">
+      <c r="B25" s="43"/>
+      <c r="C25" s="43"/>
+      <c r="D25" s="43" t="s">
+        <v>1376</v>
+      </c>
+      <c r="E25" s="44" t="s">
+        <v>1383</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5">
+      <c r="E26" s="44" t="s">
+        <v>1384</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5">
+      <c r="E27" s="44" t="s">
+        <v>1385</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5">
+      <c r="E28" s="44" t="s">
+        <v>1386</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5">
+      <c r="E29" s="44" t="s">
+        <v>1387</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5">
+      <c r="E30" s="44" t="s">
+        <v>1388</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5">
+      <c r="E31" s="44" t="s">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5">
+      <c r="E32" s="44" t="s">
+        <v>1390</v>
+      </c>
+    </row>
+    <row r="33" spans="5:5">
+      <c r="E33" s="44" t="s">
+        <v>1391</v>
+      </c>
+    </row>
+    <row r="34" spans="5:5">
+      <c r="E34" s="44" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="35" spans="5:5">
+      <c r="E35" s="44" t="s">
+        <v>1375</v>
+      </c>
+    </row>
+    <row r="36" spans="5:5">
+      <c r="E36" s="44" t="s">
+        <v>1393</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54AAEBB3-B719-46F9-94D1-46B766104A71}">
   <dimension ref="A2:A9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D34" sqref="D34"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
@@ -15480,13 +18617,14 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79A4BD8E-1932-47A2-84A6-60F94BACD786}">
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>

</xml_diff>